<commit_message>
finalizado ex 1 Dantzig
</commit_message>
<xml_diff>
--- a/exercicios/lista7/acsjunior-ppgmne-mnum7077-lista7.xlsx
+++ b/exercicios/lista7/acsjunior-ppgmne-mnum7077-lista7.xlsx
@@ -2,70 +2,122 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="EstaPastaDeTrabalho" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antonioj\Documents\personal\ppgmne-mnum7077\exercicios\lista7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B0F0AC-3012-4966-A47D-004FF72D409D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F592B8E1-AEB5-4C33-AE8C-EE45DE417A48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{06509232-7475-4E49-AEE3-E0125620DA44}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{06509232-7475-4E49-AEE3-E0125620DA44}"/>
   </bookViews>
   <sheets>
     <sheet name="Exercicio 1 (10 pts) - Dantzig" sheetId="4" r:id="rId1"/>
+    <sheet name="Exercicio 1 (10 pts) - Dant (2)" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$H$60:$K$63</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$H$60:$K$63</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$H$60:$K$63</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$H$60:$K$63</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$68:$L$81</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$H$64:$K$64</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$60:$L$63</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$60:$L$63</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$68:$L$81</definedName>
     <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$68:$L$81</definedName>
+    <definedName name="solver_lhs5" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$68:$L$81</definedName>
     <definedName name="solver_lhs5" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$68:$L$81</definedName>
+    <definedName name="solver_lhs6" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$68:$L$81</definedName>
     <definedName name="solver_lhs6" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$68:$L$81</definedName>
+    <definedName name="solver_lhs7" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$68:$L$81</definedName>
     <definedName name="solver_lhs7" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$68:$L$81</definedName>
+    <definedName name="solver_lhs8" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$68:$L$81</definedName>
     <definedName name="solver_lhs8" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$68:$L$81</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$56</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$56</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel5" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel5" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel6" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel6" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel7" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel7" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel8" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel8" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">binário</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">binário</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$N$68:$N$81</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$H$56:$K$56</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$L$52:$L$55</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$L$52:$L$55</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$N$68:$N$81</definedName>
     <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$N$68:$N$81</definedName>
+    <definedName name="solver_rhs5" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$N$68:$N$81</definedName>
     <definedName name="solver_rhs5" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$N$68:$N$81</definedName>
+    <definedName name="solver_rhs6" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$N$68:$N$81</definedName>
     <definedName name="solver_rhs6" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$N$68:$N$81</definedName>
+    <definedName name="solver_rhs7" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$N$68:$N$81</definedName>
     <definedName name="solver_rhs7" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$N$68:$N$81</definedName>
+    <definedName name="solver_rhs8" localSheetId="1" hidden="1">'Exercicio 1 (10 pts) - Dant (2)'!$N$68:$N$81</definedName>
     <definedName name="solver_rhs8" localSheetId="0" hidden="1">'Exercicio 1 (10 pts) - Dantzig'!$N$68:$N$81</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -87,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="12">
   <si>
     <t>Pontos</t>
   </si>
@@ -353,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -446,6 +498,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -474,7 +535,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -789,7 +870,328 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="pt-BR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Exercicio 1 (10 pts) - Dant (2)'!$C$51:$C$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Exercicio 1 (10 pts) - Dant (2)'!$D$51:$D$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-43C4-4F6A-B9F7-E48743436869}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="377561312"/>
+        <c:axId val="588730432"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="377561312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="588730432"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="588730432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="pt-BR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="377561312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="pt-BR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1345,6 +1747,522 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -3638,6 +4556,2321 @@
       <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="1133475" y="7724775"/>
+          <a:ext cx="3124200" cy="333375"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>33337</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>109537</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{243D4D44-6BF6-4E0E-8111-C2BA3D10CA78}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE1F65B7-6407-4CC0-B168-0AB6BECA7DCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1847850" y="838200"/>
+          <a:ext cx="1276350" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagem 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3A9BC06-936A-4B91-95B0-AE6840C48FC4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1219200" y="1924050"/>
+          <a:ext cx="1714500" cy="485775"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{235FF471-C68D-4BB1-8EC1-19F48B2C0B43}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1190625" y="2524125"/>
+          <a:ext cx="1714500" cy="504825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Imagem 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E2FBA3A-B0DF-49F8-B579-76E1C2F65777}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8143875" y="13173075"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagem 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2DDC846-3719-4D0B-A570-A36BBD216633}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8153400" y="13373100"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB1F053D-6051-4FB0-892F-D3B40EDFE0E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8162925" y="13563600"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36B32DBC-8025-427A-A74C-908FBD216C99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8162925" y="13754100"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4219CB9-5A08-440A-A991-DAE5BC924BFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8143875" y="13935075"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>71</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C052027E-1F7F-4532-B4C4-435D53F807B8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8143875" y="14125575"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20E60D37-DE1A-428C-8328-C9087D4318DF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8153400" y="14316075"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30B07E09-1127-4087-B4AC-88458C06664A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8143875" y="14516100"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagem 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1904AE03-4D6B-4E90-92D2-46B3EE636EAE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8134350" y="14706600"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagem 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7935A3B9-355B-442B-BC0B-CADAC77C08E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8124825" y="14887575"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagem 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF69A59-84F9-459B-A908-DC82741A8A99}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8134350" y="15068550"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Imagem 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C3A2732-54C1-49E3-A28C-867F9BD48886}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8134350" y="15278100"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Imagem 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08E25055-FC79-406C-8AFF-441B56ECAEDB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8143875" y="15459075"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagem 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1666D433-3D90-45AA-BFB4-C9FAD83B36E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8134350" y="15659100"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagem 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{07856704-37AA-4718-9E75-DD31F41EA4B4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1190625" y="3248025"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Imagem 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E56993F5-7868-4FF1-9C4D-208D78978D3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1190625" y="3543300"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Imagem 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CEB04DF4-F5CC-4D7D-A675-1129018426D1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="3857625"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Imagem 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{391B0891-25E9-48DA-BBD8-71962A1566D2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1181100" y="4171950"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="24" name="Imagem 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20EF9907-389B-43D0-A58D-ACA25E749EC7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="4486275"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="25" name="Imagem 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9C9A590E-BC1F-43F7-84A7-1FC46278E60A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="4810125"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Imagem 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{73FF10D0-ACD3-491A-84A1-725CBA7FA902}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1171575" y="5143500"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="27" name="Imagem 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A5A34A6F-6830-4D14-A331-4E9B36666EA1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="5448300"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Imagem 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3898FD8F-5364-4D50-BC6E-ECCF497E091F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="5772150"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="29" name="Imagem 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA5A3EF5-A6C4-423E-A390-669501A6FB13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="6115050"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="30" name="Imagem 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8C9FCF2-135F-49CE-A21F-619EBC4A6E49}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="6467475"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="31" name="Imagem 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{02B898B7-57D3-47EE-9323-6BE947B42C1F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="6791325"/>
+          <a:ext cx="1695450" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="32" name="Imagem 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E0C66789-D634-4A5E-972A-2BE7C5CFE5AA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1162050" y="7143750"/>
+          <a:ext cx="1266825" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="33" name="Imagem 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F97EFC9-691A-4E9D-83AB-D02AFAD502B3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1152525" y="7496175"/>
+          <a:ext cx="1276350" cy="180975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Imagem 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC8A589D-E4AF-4D1F-80AD-0478C549404E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19">
+          <a:clrChange>
+            <a:clrFrom>
+              <a:srgbClr val="FFFFFF"/>
+            </a:clrFrom>
+            <a:clrTo>
+              <a:srgbClr val="FFFFFF">
+                <a:alpha val="0"/>
+              </a:srgbClr>
+            </a:clrTo>
+          </a:clrChange>
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1133475" y="7934325"/>
           <a:ext cx="3124200" cy="333375"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3957,10 +7190,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FB6F7A9-F655-439F-BFD3-40C17BFE6BF0}">
+  <sheetPr codeName="Planilha1"/>
   <dimension ref="B2:N81"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="N45" sqref="N45"/>
+    <sheetView showGridLines="0" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3970,19 +7204,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="L2" s="41"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B5" s="25" t="s">
@@ -3995,19 +7229,19 @@
       </c>
     </row>
     <row r="47" spans="2:12" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="B47" s="41" t="s">
+      <c r="B47" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="C47" s="41"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
-      <c r="F47" s="41"/>
-      <c r="G47" s="41"/>
-      <c r="H47" s="41"/>
-      <c r="I47" s="41"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="41"/>
-      <c r="L47" s="41"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B50" s="10" t="s">
@@ -4019,10 +7253,10 @@
       <c r="D50" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F50" s="34" t="s">
+      <c r="F50" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="G50" s="35"/>
+      <c r="G50" s="38"/>
       <c r="H50" s="19">
         <v>20</v>
       </c>
@@ -4046,8 +7280,8 @@
       <c r="D51" s="7">
         <v>76</v>
       </c>
-      <c r="F51" s="36"/>
-      <c r="G51" s="37"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="40"/>
       <c r="H51" s="21">
         <v>43</v>
       </c>
@@ -4353,11 +7587,11 @@
       <c r="K67" s="14">
         <v>4</v>
       </c>
-      <c r="L67" s="38" t="s">
+      <c r="L67" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="M67" s="39"/>
-      <c r="N67" s="40"/>
+      <c r="M67" s="42"/>
+      <c r="N67" s="43"/>
     </row>
     <row r="68" spans="4:14" x14ac:dyDescent="0.25">
       <c r="G68" s="28"/>
@@ -4715,6 +7949,783 @@
     <mergeCell ref="L67:N67"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B47:L47"/>
+  </mergeCells>
+  <conditionalFormatting sqref="H68:K81">
+    <cfRule type="cellIs" dxfId="3" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H60:K63">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C830764B-8F23-4862-BA43-1234E5B381DE}">
+  <sheetPr codeName="Planilha2"/>
+  <dimension ref="B2:N81"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="L56" sqref="L56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B2" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B5" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B9" s="25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12" ht="31.5" x14ac:dyDescent="0.5">
+      <c r="B47" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="44"/>
+    </row>
+    <row r="50" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B50" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D50" s="36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F50" s="37" t="s">
+        <v>3</v>
+      </c>
+      <c r="G50" s="38"/>
+      <c r="H50" s="19">
+        <v>20</v>
+      </c>
+      <c r="I50" s="19">
+        <v>48</v>
+      </c>
+      <c r="J50" s="19">
+        <v>43</v>
+      </c>
+      <c r="K50" s="20">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="51" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B51" s="11">
+        <v>1</v>
+      </c>
+      <c r="C51" s="6">
+        <v>36</v>
+      </c>
+      <c r="D51" s="7">
+        <v>76</v>
+      </c>
+      <c r="F51" s="39"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="21">
+        <v>43</v>
+      </c>
+      <c r="I51" s="21">
+        <v>67</v>
+      </c>
+      <c r="J51" s="21">
+        <v>93</v>
+      </c>
+      <c r="K51" s="18">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B52" s="11">
+        <v>2</v>
+      </c>
+      <c r="C52" s="6">
+        <v>16</v>
+      </c>
+      <c r="D52" s="7">
+        <v>42</v>
+      </c>
+      <c r="F52" s="15">
+        <v>20</v>
+      </c>
+      <c r="G52" s="16">
+        <v>43</v>
+      </c>
+      <c r="H52" s="2">
+        <f>SQRT(($F52-H$50)^2+($G52-H$51)^2)</f>
+        <v>0</v>
+      </c>
+      <c r="I52" s="2">
+        <f t="shared" ref="I52:K55" si="0">SQRT(($F52-I$50)^2+($G52-I$51)^2)</f>
+        <v>36.878177829171548</v>
+      </c>
+      <c r="J52" s="2">
+        <f t="shared" si="0"/>
+        <v>55.036351623268054</v>
+      </c>
+      <c r="K52" s="3">
+        <f t="shared" si="0"/>
+        <v>13.601470508735444</v>
+      </c>
+      <c r="L52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B53" s="11">
+        <v>3</v>
+      </c>
+      <c r="C53" s="6">
+        <v>57</v>
+      </c>
+      <c r="D53" s="7">
+        <v>58</v>
+      </c>
+      <c r="F53" s="15">
+        <v>48</v>
+      </c>
+      <c r="G53" s="16">
+        <v>67</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" ref="H53:H55" si="1">SQRT(($F53-H$50)^2+($G53-H$51)^2)</f>
+        <v>36.878177829171548</v>
+      </c>
+      <c r="I53" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="2">
+        <f t="shared" si="0"/>
+        <v>26.476404589747453</v>
+      </c>
+      <c r="K53" s="3">
+        <f t="shared" si="0"/>
+        <v>33.837848631377263</v>
+      </c>
+      <c r="L53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B54" s="12">
+        <v>4</v>
+      </c>
+      <c r="C54" s="8">
+        <v>50</v>
+      </c>
+      <c r="D54" s="9">
+        <v>74</v>
+      </c>
+      <c r="F54" s="15">
+        <v>43</v>
+      </c>
+      <c r="G54" s="16">
+        <v>93</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>55.036351623268054</v>
+      </c>
+      <c r="I54" s="2">
+        <f t="shared" si="0"/>
+        <v>26.476404589747453</v>
+      </c>
+      <c r="J54" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K54" s="3">
+        <f t="shared" si="0"/>
+        <v>45.803929962395145</v>
+      </c>
+      <c r="L54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="F55" s="17">
+        <v>16</v>
+      </c>
+      <c r="G55" s="18">
+        <v>56</v>
+      </c>
+      <c r="H55" s="4">
+        <f t="shared" si="1"/>
+        <v>13.601470508735444</v>
+      </c>
+      <c r="I55" s="4">
+        <f t="shared" si="0"/>
+        <v>33.837848631377263</v>
+      </c>
+      <c r="J55" s="4">
+        <f t="shared" si="0"/>
+        <v>45.803929962395145</v>
+      </c>
+      <c r="K55" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+      <c r="I56" s="1">
+        <v>1</v>
+      </c>
+      <c r="J56" s="1">
+        <v>1</v>
+      </c>
+      <c r="K56" s="1">
+        <v>1</v>
+      </c>
+      <c r="L56" s="24">
+        <f>SUMPRODUCT(H60:K63,H52:K55)</f>
+        <v>122.75998289004959</v>
+      </c>
+    </row>
+    <row r="57" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="D57" s="23"/>
+    </row>
+    <row r="59" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G59" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H59" s="34">
+        <v>1</v>
+      </c>
+      <c r="I59" s="35">
+        <v>2</v>
+      </c>
+      <c r="J59" s="35">
+        <v>3</v>
+      </c>
+      <c r="K59" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G60" s="11">
+        <v>1</v>
+      </c>
+      <c r="H60" s="6">
+        <v>0</v>
+      </c>
+      <c r="I60" s="6">
+        <v>0</v>
+      </c>
+      <c r="J60" s="6">
+        <v>0</v>
+      </c>
+      <c r="K60" s="7">
+        <v>1</v>
+      </c>
+      <c r="L60" s="1">
+        <f>SUM(H60:K60)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G61" s="11">
+        <v>2</v>
+      </c>
+      <c r="H61" s="6">
+        <v>1</v>
+      </c>
+      <c r="I61" s="6">
+        <v>0</v>
+      </c>
+      <c r="J61" s="6">
+        <v>0</v>
+      </c>
+      <c r="K61" s="7">
+        <v>0</v>
+      </c>
+      <c r="L61" s="1">
+        <f t="shared" ref="L61:L63" si="2">SUM(H61:K61)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G62" s="11">
+        <v>3</v>
+      </c>
+      <c r="H62" s="6">
+        <v>0</v>
+      </c>
+      <c r="I62" s="6">
+        <v>1</v>
+      </c>
+      <c r="J62" s="6">
+        <v>0</v>
+      </c>
+      <c r="K62" s="7">
+        <v>0</v>
+      </c>
+      <c r="L62" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="G63" s="12">
+        <v>4</v>
+      </c>
+      <c r="H63" s="8">
+        <v>0</v>
+      </c>
+      <c r="I63" s="8">
+        <v>0</v>
+      </c>
+      <c r="J63" s="8">
+        <v>1</v>
+      </c>
+      <c r="K63" s="9">
+        <v>0</v>
+      </c>
+      <c r="L63" s="1">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="H64" s="1">
+        <f>SUM(H60:H63)</f>
+        <v>1</v>
+      </c>
+      <c r="I64" s="1">
+        <f t="shared" ref="I64:K64" si="3">SUM(I60:I63)</f>
+        <v>1</v>
+      </c>
+      <c r="J64" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K64" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D67" s="23"/>
+      <c r="G67" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="H67" s="34">
+        <v>1</v>
+      </c>
+      <c r="I67" s="35">
+        <v>2</v>
+      </c>
+      <c r="J67" s="35">
+        <v>3</v>
+      </c>
+      <c r="K67" s="36">
+        <v>4</v>
+      </c>
+      <c r="L67" s="41" t="s">
+        <v>6</v>
+      </c>
+      <c r="M67" s="42"/>
+      <c r="N67" s="43"/>
+    </row>
+    <row r="68" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G68" s="28"/>
+      <c r="H68" s="26">
+        <v>1</v>
+      </c>
+      <c r="I68" s="6">
+        <v>0</v>
+      </c>
+      <c r="J68" s="6">
+        <v>0</v>
+      </c>
+      <c r="K68" s="7">
+        <v>0</v>
+      </c>
+      <c r="L68" s="30">
+        <f>I60+J60+K60</f>
+        <v>1</v>
+      </c>
+      <c r="M68" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N68" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G69" s="28"/>
+      <c r="H69" s="26">
+        <v>0</v>
+      </c>
+      <c r="I69" s="6">
+        <v>1</v>
+      </c>
+      <c r="J69" s="6">
+        <v>0</v>
+      </c>
+      <c r="K69" s="7">
+        <v>0</v>
+      </c>
+      <c r="L69" s="30">
+        <f>H61+J61+K61</f>
+        <v>1</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N69" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G70" s="28"/>
+      <c r="H70" s="26">
+        <v>1</v>
+      </c>
+      <c r="I70" s="6">
+        <v>1</v>
+      </c>
+      <c r="J70" s="6">
+        <v>0</v>
+      </c>
+      <c r="K70" s="7">
+        <v>0</v>
+      </c>
+      <c r="L70" s="30">
+        <f>J60+K60+J61+K61</f>
+        <v>1</v>
+      </c>
+      <c r="M70" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N70" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G71" s="28"/>
+      <c r="H71" s="26">
+        <v>0</v>
+      </c>
+      <c r="I71" s="6">
+        <v>0</v>
+      </c>
+      <c r="J71" s="6">
+        <v>1</v>
+      </c>
+      <c r="K71" s="7">
+        <v>0</v>
+      </c>
+      <c r="L71" s="30">
+        <f>H62+I62+K62</f>
+        <v>1</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N71" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G72" s="28"/>
+      <c r="H72" s="26">
+        <v>1</v>
+      </c>
+      <c r="I72" s="6">
+        <v>0</v>
+      </c>
+      <c r="J72" s="6">
+        <v>1</v>
+      </c>
+      <c r="K72" s="7">
+        <v>0</v>
+      </c>
+      <c r="L72" s="30">
+        <f>I60+K60+I62+K62</f>
+        <v>2</v>
+      </c>
+      <c r="M72" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N72" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G73" s="28"/>
+      <c r="H73" s="26">
+        <v>0</v>
+      </c>
+      <c r="I73" s="6">
+        <v>1</v>
+      </c>
+      <c r="J73" s="6">
+        <v>1</v>
+      </c>
+      <c r="K73" s="7">
+        <v>0</v>
+      </c>
+      <c r="L73" s="30">
+        <f>H61+K61+H62+K62</f>
+        <v>1</v>
+      </c>
+      <c r="M73" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N73" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G74" s="28"/>
+      <c r="H74" s="26">
+        <v>1</v>
+      </c>
+      <c r="I74" s="6">
+        <v>1</v>
+      </c>
+      <c r="J74" s="6">
+        <v>1</v>
+      </c>
+      <c r="K74" s="7">
+        <v>0</v>
+      </c>
+      <c r="L74" s="30">
+        <f>K60+K61+K62</f>
+        <v>1</v>
+      </c>
+      <c r="M74" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N74" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G75" s="28"/>
+      <c r="H75" s="26">
+        <v>0</v>
+      </c>
+      <c r="I75" s="6">
+        <v>0</v>
+      </c>
+      <c r="J75" s="6">
+        <v>0</v>
+      </c>
+      <c r="K75" s="7">
+        <v>1</v>
+      </c>
+      <c r="L75" s="30">
+        <f>H63+I63+J63</f>
+        <v>1</v>
+      </c>
+      <c r="M75" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N75" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G76" s="28"/>
+      <c r="H76" s="26">
+        <v>1</v>
+      </c>
+      <c r="I76" s="6">
+        <v>0</v>
+      </c>
+      <c r="J76" s="6">
+        <v>0</v>
+      </c>
+      <c r="K76" s="7">
+        <v>1</v>
+      </c>
+      <c r="L76" s="30">
+        <f>I60+J60+I63+J63</f>
+        <v>1</v>
+      </c>
+      <c r="M76" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N76" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G77" s="28"/>
+      <c r="H77" s="26">
+        <v>0</v>
+      </c>
+      <c r="I77" s="6">
+        <v>1</v>
+      </c>
+      <c r="J77" s="6">
+        <v>0</v>
+      </c>
+      <c r="K77" s="7">
+        <v>1</v>
+      </c>
+      <c r="L77" s="30">
+        <f>H61+J61+H63+J63</f>
+        <v>2</v>
+      </c>
+      <c r="M77" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N77" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G78" s="28"/>
+      <c r="H78" s="26">
+        <v>1</v>
+      </c>
+      <c r="I78" s="6">
+        <v>1</v>
+      </c>
+      <c r="J78" s="6">
+        <v>0</v>
+      </c>
+      <c r="K78" s="7">
+        <v>1</v>
+      </c>
+      <c r="L78" s="30">
+        <f>J60+J61+J63</f>
+        <v>1</v>
+      </c>
+      <c r="M78" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N78" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G79" s="28"/>
+      <c r="H79" s="26">
+        <v>0</v>
+      </c>
+      <c r="I79" s="6">
+        <v>0</v>
+      </c>
+      <c r="J79" s="6">
+        <v>1</v>
+      </c>
+      <c r="K79" s="7">
+        <v>1</v>
+      </c>
+      <c r="L79" s="30">
+        <f>H62+I62+H63+I63</f>
+        <v>1</v>
+      </c>
+      <c r="M79" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N79" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="G80" s="28"/>
+      <c r="H80" s="26">
+        <v>1</v>
+      </c>
+      <c r="I80" s="6">
+        <v>0</v>
+      </c>
+      <c r="J80" s="6">
+        <v>1</v>
+      </c>
+      <c r="K80" s="7">
+        <v>1</v>
+      </c>
+      <c r="L80" s="30">
+        <f>I60+I62+I63</f>
+        <v>1</v>
+      </c>
+      <c r="M80" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N80" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G81" s="29"/>
+      <c r="H81" s="27">
+        <v>0</v>
+      </c>
+      <c r="I81" s="8">
+        <v>1</v>
+      </c>
+      <c r="J81" s="8">
+        <v>1</v>
+      </c>
+      <c r="K81" s="9">
+        <v>1</v>
+      </c>
+      <c r="L81" s="31">
+        <f>H61+H62+H63</f>
+        <v>1</v>
+      </c>
+      <c r="M81" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="N81" s="33">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="F50:G51"/>
+    <mergeCell ref="L67:N67"/>
   </mergeCells>
   <conditionalFormatting sqref="H68:K81">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>